<commit_message>
Caso de teste de busca por categoria
</commit_message>
<xml_diff>
--- a/src/test/java/br/com/rsinet/HUB_BDD/testData/BancoDados.xlsx
+++ b/src/test/java/br/com/rsinet/HUB_BDD/testData/BancoDados.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abdiel.cordeiro\Documents\Projetos\eclipse-workspace\projetoTDD\src\br\com\rsinet\HUB_TDD\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abdiel.cordeiro\Documents\Projetos\eclipse-workspace\projetoBDD\src\test\java\br\com\rsinet\HUB_BDD\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FD83952-37E0-4BB7-B620-8F4F90083EF7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9665C828-C1A9-4585-B827-BAC014E82BB7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C4F5F6C9-57A0-43D3-9FA4-F5EF18E402B6}"/>
   </bookViews>
@@ -32,19 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
-  <si>
-    <t>userName</t>
-  </si>
-  <si>
-    <t>userPass</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>FristName</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
   <si>
     <t>LastName</t>
   </si>
@@ -61,18 +49,12 @@
     <t>Cordeiro</t>
   </si>
   <si>
-    <t>phoneNumber</t>
-  </si>
-  <si>
     <t>City</t>
   </si>
   <si>
     <t>Osasco</t>
   </si>
   <si>
-    <t>address</t>
-  </si>
-  <si>
     <t>Rua Antonio Bertoldo de Oliveira</t>
   </si>
   <si>
@@ -82,9 +64,6 @@
     <t>São Paulo</t>
   </si>
   <si>
-    <t>CEP</t>
-  </si>
-  <si>
     <t>06290-060</t>
   </si>
   <si>
@@ -103,9 +82,6 @@
     <t>HP USB 3 Button Optical Mouse</t>
   </si>
   <si>
-    <t>Pais</t>
-  </si>
-  <si>
     <t>Brazil</t>
   </si>
   <si>
@@ -139,7 +115,37 @@
     <t>Mochila</t>
   </si>
   <si>
-    <t>lucasViado</t>
+    <t>lucasViadoadasdda</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>PostalCode</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>UserNameFalha</t>
+  </si>
+  <si>
+    <t>UserPass</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>PhoneNumber</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>lucasVi</t>
   </si>
 </sst>
 </file>
@@ -537,112 +543,127 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D6D5505-1405-49EC-A52B-B536267B1E1D}">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" style="2"/>
-    <col min="8" max="8" width="28.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="8.88671875" style="2"/>
-    <col min="11" max="11" width="16.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.88671875" style="2"/>
+    <col min="2" max="2" width="16.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" style="2"/>
+    <col min="9" max="9" width="28.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.88671875" style="2"/>
+    <col min="11" max="11" width="10.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>9</v>
-      </c>
       <c r="G1" s="3" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="L1" s="3"/>
+        <v>29</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
-      <c r="O1" s="1"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O1" s="3"/>
+      <c r="P1" s="1"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>11</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="L2" s="4"/>
+        <v>10</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O2" s="4"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="6"/>
-      <c r="K3" s="7"/>
+      <c r="B3" s="6"/>
+      <c r="L3" s="7"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="D5" s="6"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K7" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{46AC47A1-1F89-45AF-8C7B-F4A195208066}"/>
-    <hyperlink ref="C2" r:id="rId2" xr:uid="{85BD8E5A-7C04-41EF-BADE-536F55EA589D}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{46AC47A1-1F89-45AF-8C7B-F4A195208066}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{85BD8E5A-7C04-41EF-BADE-536F55EA589D}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
@@ -666,73 +687,73 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Configuração do extendReport no BDD
</commit_message>
<xml_diff>
--- a/src/test/java/br/com/rsinet/HUB_BDD/testData/BancoDados.xlsx
+++ b/src/test/java/br/com/rsinet/HUB_BDD/testData/BancoDados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abdiel.cordeiro\Documents\Projetos\eclipse-workspace\projetoBDD\src\test\java\br\com\rsinet\HUB_BDD\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CA5C3C1-27CD-4BC8-82EF-00EE1DF87F02}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D7EF7D1-5F29-4795-BA90-7AC0106AC082}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{C4F5F6C9-57A0-43D3-9FA4-F5EF18E402B6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C4F5F6C9-57A0-43D3-9FA4-F5EF18E402B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Cadastro" sheetId="1" r:id="rId1"/>
@@ -142,7 +142,7 @@
     <t>Address</t>
   </si>
   <si>
-    <t>lucasVi</t>
+    <t>abdielCor</t>
   </si>
 </sst>
 </file>
@@ -542,8 +542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D6D5505-1405-49EC-A52B-B536267B1E1D}">
   <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -671,7 +671,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB9334BD-5787-4860-8F04-DE32560FFDB3}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Ajuste na criação do arquivo do reporte
</commit_message>
<xml_diff>
--- a/src/test/java/br/com/rsinet/HUB_BDD/testData/BancoDados.xlsx
+++ b/src/test/java/br/com/rsinet/HUB_BDD/testData/BancoDados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abdiel.cordeiro\Documents\Projetos\eclipse-workspace\projetoBDD\src\test\java\br\com\rsinet\HUB_BDD\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D7EF7D1-5F29-4795-BA90-7AC0106AC082}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F67412D3-9CFB-467D-80FC-9F94A5EB1FB0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C4F5F6C9-57A0-43D3-9FA4-F5EF18E402B6}"/>
   </bookViews>
@@ -142,7 +142,7 @@
     <t>Address</t>
   </si>
   <si>
-    <t>abdielCor</t>
+    <t>abdielCordei</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Ajustes na massa de dados e nos teste de falha de clique
</commit_message>
<xml_diff>
--- a/src/test/java/br/com/rsinet/HUB_BDD/testData/BancoDados.xlsx
+++ b/src/test/java/br/com/rsinet/HUB_BDD/testData/BancoDados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abdiel.cordeiro\Documents\Projetos\eclipse-workspace\projetoBDD\src\test\java\br\com\rsinet\HUB_BDD\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F67412D3-9CFB-467D-80FC-9F94A5EB1FB0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32D3E444-45FA-4A59-91C6-162A7DAFE858}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C4F5F6C9-57A0-43D3-9FA4-F5EF18E402B6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{C4F5F6C9-57A0-43D3-9FA4-F5EF18E402B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Cadastro" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
   <si>
     <t>LastName</t>
   </si>
@@ -143,6 +143,9 @@
   </si>
   <si>
     <t>abdielCordei</t>
+  </si>
+  <si>
+    <t>Quantidade</t>
   </si>
 </sst>
 </file>
@@ -206,7 +209,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -224,6 +227,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -542,7 +548,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D6D5505-1405-49EC-A52B-B536267B1E1D}">
   <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -671,15 +677,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB9334BD-5787-4860-8F04-DE32560FFDB3}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="2"/>
     <col min="2" max="2" width="36.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="2"/>
+    <col min="3" max="4" width="8.88671875" style="2"/>
+    <col min="5" max="5" width="10.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -692,6 +700,9 @@
       <c r="C1" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="E1" s="3" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
@@ -701,6 +712,9 @@
         <v>17</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="9">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adicionado os comentarios e after e before
</commit_message>
<xml_diff>
--- a/src/test/java/br/com/rsinet/HUB_BDD/testData/BancoDados.xlsx
+++ b/src/test/java/br/com/rsinet/HUB_BDD/testData/BancoDados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abdiel.cordeiro\Documents\Projetos\eclipse-workspace\projetoBDD\src\test\java\br\com\rsinet\HUB_BDD\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32D3E444-45FA-4A59-91C6-162A7DAFE858}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDF4FA8E-C959-4EF2-A36C-9FD62D1963A4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{C4F5F6C9-57A0-43D3-9FA4-F5EF18E402B6}"/>
   </bookViews>
@@ -678,7 +678,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Ajustes no codigo com a classe before
</commit_message>
<xml_diff>
--- a/src/test/java/br/com/rsinet/HUB_BDD/testData/BancoDados.xlsx
+++ b/src/test/java/br/com/rsinet/HUB_BDD/testData/BancoDados.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abdiel.cordeiro\Documents\Projetos\eclipse-workspace\projetoBDD\src\test\java\br\com\rsinet\HUB_BDD\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDF4FA8E-C959-4EF2-A36C-9FD62D1963A4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D0E49E4-6F21-4142-96C0-EA31904086A9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{C4F5F6C9-57A0-43D3-9FA4-F5EF18E402B6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C4F5F6C9-57A0-43D3-9FA4-F5EF18E402B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Cadastro" sheetId="1" r:id="rId1"/>
@@ -142,10 +142,10 @@
     <t>Address</t>
   </si>
   <si>
-    <t>abdielCordei</t>
-  </si>
-  <si>
     <t>Quantidade</t>
+  </si>
+  <si>
+    <t>3abdielCordei4</t>
   </si>
 </sst>
 </file>
@@ -548,7 +548,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D6D5505-1405-49EC-A52B-B536267B1E1D}">
   <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -613,7 +613,7 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>26</v>
@@ -677,7 +677,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB9334BD-5787-4860-8F04-DE32560FFDB3}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
@@ -701,7 +701,7 @@
         <v>19</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>